<commit_message>
modify excel export begin point
</commit_message>
<xml_diff>
--- a/src/main/resources/SH688126.xlsx
+++ b/src/main/resources/SH688126.xlsx
@@ -74,40 +74,30 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>20200424</t>
+          <t>20200714</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1071.0</v>
+        <v>6900.0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>20200714</t>
+          <t>20200724</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>6900.0</v>
+        <v>3700.0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>20200724</t>
+          <t>20200805</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>3700.0</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>20200805</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
         <v>5960.0</v>
       </c>
     </row>

</xml_diff>